<commit_message>
wip: avancement sur la maquette; add: client page maquette; add: projects page maquette
</commit_message>
<xml_diff>
--- a/documentation/Planning_final_TPI_intro-Luca_Maggioli.xlsx
+++ b/documentation/Planning_final_TPI_intro-Luca_Maggioli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nagragrp-my.sharepoint.com/personal/luca_maggioli_nagra_com/Documents/Desktop/Apprentissage/TPI_intro/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{E21018F4-C4DA-43D7-98A4-DF276D51E0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7488A4D-5AC8-43F4-9325-492465D9544F}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{E21018F4-C4DA-43D7-98A4-DF276D51E0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C06F70B7-3853-4F6A-B2E6-4EF63E3282BE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F6868423-5B24-42CE-9158-947897399ED9}"/>
   </bookViews>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CA3C5D-4C1F-4C60-BF94-C9399AC6FD5D}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -731,8 +731,8 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>

</xml_diff>